<commit_message>
updated documentation before optics_r001 is sent to fab
</commit_message>
<xml_diff>
--- a/doc/design/bom.xlsx
+++ b/doc/design/bom.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="350">
   <si>
     <t>MFR</t>
   </si>
@@ -875,6 +875,210 @@
   </si>
   <si>
     <t>TOL (%)</t>
+  </si>
+  <si>
+    <t>Hitec Servo</t>
+  </si>
+  <si>
+    <t>http://www.semiconductorstore.com/cart/pc/viewPrd.asp?idproduct=41773</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Molex/22-28-4030/?qs=%2fha2pyFaduguMWEp6M%252bj06c%2f9D%252bCJj2JzpHwCqFruQ0%3d</t>
+  </si>
+  <si>
+    <t>X4, X5</t>
+  </si>
+  <si>
+    <t>DS5, DS7</t>
+  </si>
+  <si>
+    <t>DS3, DS6</t>
+  </si>
+  <si>
+    <t>DS1, DS4, DS8</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Molex/90120-0130/?qs=%2fha2pyFadujqg59qjGW4yJgp9NLYVsw150yd8op0CsE%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Kingbright/APT3216QBC-D/?qs=%2fha2pyFaduiVG4P3QLv39v40xPBnyxjjHntlVha2SjZA%252b0kB9quO7Q%3d%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Kingbright/APT3216SURCK/?qs=%2fha2pyFaduhU1pKkAWLu%2f2tBFgOVVOW7IvaSTApofs8L82sNR3fhUQ%3d%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Kingbright/APT3216SYCK/?qs=sGAEpiMZZMseGfSY3csMkeytxqHAv00AregDridya2g%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Cree-Inc/C503B-BCN-CV0Z0461/?qs=%2fha2pyFadugFm5YULr%252bT3V4eaaImD7nw663PqqPaPl%252bDsPv%252bXnXdKMuRS2ED%2foVN</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Molex/90147-1108/?qs=%2fha2pyFaduhzmffJ8xf3YDdKsDd5Jl43YS3FyK9Z1rg%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay/SI2342DS-T1-GE3/?qs=%2fha2pyFaduiOdPcVz1SkCaU%252bgfGeShrTZkgvoEQN4mk%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay/SI2333DDS-T1-GE3/?qs=%2fha2pyFaduiN0OWuAS8wJRS0NDLMAm1g4oXA6hzxovg%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/OSRAM-Opto-Semiconductors/PL-450B/?qs=sGAEpiMZZMsgNhPy3wz0s9My9cyTx8s8tIn5WHR65S8%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/First-Sensor/QP10-6-TO5/?qs=%2fha2pyFaduj2fRtOGGJwMemZr7UkdRMhmXfy2L0GivE%3d</t>
+  </si>
+  <si>
+    <t>VJ0805A101GXAPW1BC</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay-Vitramon/VJ0805A101GXAPW1BC/?qs=sGAEpiMZZMs0AnBnWHyRQGchlqIXPxeo1mYIMQMQF3Q%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay-Vitramon/VJ0805A222GXACW1BC/?qs=sGAEpiMZZMs0AnBnWHyRQGuekufMepD5djjdV3uhZnU%3d</t>
+  </si>
+  <si>
+    <t>VJ0805A222GXACW1BC</t>
+  </si>
+  <si>
+    <t>C/2%/0805/10V</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay-Vitramon/VJ0805A2R2BXAPW1BC/?qs=sGAEpiMZZMs0AnBnWHyRQKsgPTXVq8S74jYR%252bqOURhg%3d</t>
+  </si>
+  <si>
+    <t>VJ0805A2R2BXAPW1BC</t>
+  </si>
+  <si>
+    <t>C/20%/0805/10V</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay-Vitramon/VJ0805V105MXJCW1BC/?qs=sGAEpiMZZMs0AnBnWHyRQKsgPTXVq8S7svovNV5aCMo%3d</t>
+  </si>
+  <si>
+    <t>VJ0805V105MXJCW1BC</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay-Vitramon/VJ0805Y104JXXAC/?qs=sGAEpiMZZMs0AnBnWHyRQKubRBCdVSJlNb%252b2LWoQTfI%3d</t>
+  </si>
+  <si>
+    <t>VJ0805Y104JXXAC</t>
+  </si>
+  <si>
+    <t>VJ0805Y472JXXCW1BC</t>
+  </si>
+  <si>
+    <t>CRCW08050000Z0EA</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay/CRCW0805100RFKEA/?qs=sGAEpiMZZMvdGkrng054txEw7b1YnvGuUG%2fFwliasrw%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay/CRCW08050000Z0EA/?qs=sGAEpiMZZMvdGkrng054t1VbmbR8V6nMvsgH2bmS3m0%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay/CRCW080510K0FKEA/?qs=sGAEpiMZZMvdGkrng054txEw7b1YnvGub0TWhH3fIZU%3d</t>
+  </si>
+  <si>
+    <t>CRCW080510K0FKEA</t>
+  </si>
+  <si>
+    <t>CRCW0805100RFKEA</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay/CRCW0805137RFKEA/?qs=sGAEpiMZZMvdGkrng054tygjBeyq%2fOAOObaXM7l7UWU%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay/CRCW0805150RFKEA/?qs=sGAEpiMZZMvdGkrng054txEw7b1YnvGu7FNBL7MPgY4%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay/CRCW080522K0FKEA/?qs=sGAEpiMZZMvdGkrng054tygjBeyq%2fOAOcSGHQ3E9G%2fA%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay/CRCW08054K70FKEA/?qs=sGAEpiMZZMvdGkrng054txEw7b1YnvGuPN5czM2Dtwg%3d</t>
+  </si>
+  <si>
+    <t>CRCW0805137RFKEA</t>
+  </si>
+  <si>
+    <t>CRCW08054K70FKEA</t>
+  </si>
+  <si>
+    <t>CRCW0805150RFKEA</t>
+  </si>
+  <si>
+    <t>CRCW080522K0FKEA</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay/CRCW080568R0FKEA/?qs=sGAEpiMZZMvdGkrng054tygjBeyq%2fOAOqqZ8HLKft38%3d</t>
+  </si>
+  <si>
+    <t>CRCW080582R0FKEA</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay/CRCW080580R6FKEA/?qs=sGAEpiMZZMvdGkrng054tygjBeyq%2fOAOZF%2fgGLYZzqU%3d</t>
+  </si>
+  <si>
+    <t>CRCW080580R6FKEA</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay/T93YB103KT20/?qs=%2fha2pyFaduiy5ZPEGg5ujJikQNwEmb4%252bmBoyiWZ0AW276Z%2f76g9nrA%3d%3d</t>
+  </si>
+  <si>
+    <t>RCWE1206R820FKEA</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay-Dale/RCWE1206R820FKEA/?qs=sGAEpiMZZMtlleCFQhR%2fzWNMMPf0rCM7CsJq3yiQ0CM%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay-Vitramon/VJ0805Y473JXAPW1BC/?qs=sGAEpiMZZMs0AnBnWHyRQGuekufMepD58Ioe0rxjtIc%3d</t>
+  </si>
+  <si>
+    <t>100pF</t>
+  </si>
+  <si>
+    <t>2.2nF</t>
+  </si>
+  <si>
+    <t>2pF</t>
+  </si>
+  <si>
+    <t>1uF</t>
+  </si>
+  <si>
+    <t>0.1uF</t>
+  </si>
+  <si>
+    <t>47nF</t>
+  </si>
+  <si>
+    <t>0Ω</t>
+  </si>
+  <si>
+    <t>100Ω</t>
+  </si>
+  <si>
+    <t>10kΩ</t>
+  </si>
+  <si>
+    <t>137Ω</t>
+  </si>
+  <si>
+    <t>150Ω</t>
+  </si>
+  <si>
+    <t>22kΩ</t>
+  </si>
+  <si>
+    <t>4.7kΩ</t>
+  </si>
+  <si>
+    <t>68Ω</t>
+  </si>
+  <si>
+    <t>80.6Ω</t>
+  </si>
+  <si>
+    <t>0.82Ω</t>
   </si>
 </sst>
 </file>
@@ -998,7 +1202,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1127,6 +1331,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -2394,39 +2601,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L7"/>
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="35.4609375" customWidth="1"/>
+    <col min="1" max="1" width="28.3828125" customWidth="1"/>
     <col min="2" max="2" width="8.15234375" customWidth="1"/>
-    <col min="3" max="3" width="8.61328125" customWidth="1"/>
-    <col min="4" max="4" width="6" customWidth="1"/>
+    <col min="3" max="3" width="8.61328125" style="46" customWidth="1"/>
+    <col min="4" max="4" width="7.921875" style="46" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.3828125" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
     <col min="8" max="8" width="24.61328125" customWidth="1"/>
-    <col min="9" max="9" width="11.53515625" style="43" customWidth="1"/>
-    <col min="10" max="10" width="10.4609375" customWidth="1"/>
-    <col min="11" max="11" width="4.07421875" customWidth="1"/>
-    <col min="12" max="12" width="28.07421875" customWidth="1"/>
+    <col min="9" max="9" width="15.765625" customWidth="1"/>
+    <col min="10" max="10" width="9.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="41" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" s="41" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="40" t="s">
         <v>100</v>
       </c>
       <c r="E1" s="40" t="s">
@@ -2441,25 +2646,32 @@
       <c r="H1" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="42" t="s">
-        <v>140</v>
+      <c r="I1" s="4" t="s">
+        <v>141</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>255</v>
+        <v>303</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="C2" s="45">
+        <v>0.1</v>
+      </c>
+      <c r="D2" s="45">
+        <f>B2*C2</f>
+        <v>0.8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" t="s">
+        <v>299</v>
       </c>
       <c r="G2" t="s">
         <v>256</v>
@@ -2467,23 +2679,32 @@
       <c r="H2" t="s">
         <v>153</v>
       </c>
-      <c r="I2" s="43" t="s">
-        <v>157</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2" t="str">
-        <f>I2&amp;"F"</f>
-        <v>100pF</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="I2" t="s">
+        <v>334</v>
+      </c>
+      <c r="J2" s="44" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>255</v>
+        <v>303</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C3" s="45">
+        <v>0.18</v>
+      </c>
+      <c r="D3" s="45">
+        <f t="shared" ref="D3:D32" si="0">B3*C3</f>
+        <v>0.36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" t="s">
+        <v>302</v>
       </c>
       <c r="G3" t="s">
         <v>165</v>
@@ -2491,23 +2712,32 @@
       <c r="H3" t="s">
         <v>153</v>
       </c>
-      <c r="I3" s="43" t="s">
-        <v>164</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3" t="str">
-        <f t="shared" ref="L3:L7" si="0">I3&amp;"F"</f>
-        <v>2.2nF</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="I3" t="s">
+        <v>335</v>
+      </c>
+      <c r="J3" s="44" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>255</v>
+        <v>303</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="C4" s="45">
+        <v>0.1</v>
+      </c>
+      <c r="D4" s="45">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" t="s">
+        <v>305</v>
       </c>
       <c r="G4" t="s">
         <v>262</v>
@@ -2515,23 +2745,32 @@
       <c r="H4" t="s">
         <v>153</v>
       </c>
-      <c r="I4" s="43" t="s">
-        <v>168</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4" t="str">
+      <c r="I4" t="s">
+        <v>336</v>
+      </c>
+      <c r="J4" s="44" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>306</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="45">
+        <v>0.23</v>
+      </c>
+      <c r="D5" s="45">
         <f t="shared" si="0"/>
-        <v>2pF</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>261</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
+        <v>0.46</v>
+      </c>
+      <c r="E5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" t="s">
+        <v>308</v>
       </c>
       <c r="G5" t="s">
         <v>163</v>
@@ -2539,23 +2778,32 @@
       <c r="H5" t="s">
         <v>153</v>
       </c>
-      <c r="I5" s="43" t="s">
-        <v>162</v>
-      </c>
-      <c r="K5">
-        <v>10</v>
-      </c>
-      <c r="L5" t="str">
-        <f t="shared" si="0"/>
-        <v>1uF</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="I5" t="s">
+        <v>337</v>
+      </c>
+      <c r="J5" s="44" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>252</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C6" s="45">
+        <v>0.1</v>
+      </c>
+      <c r="D6" s="45">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" t="s">
+        <v>310</v>
       </c>
       <c r="G6" t="s">
         <v>156</v>
@@ -2563,23 +2811,32 @@
       <c r="H6" t="s">
         <v>153</v>
       </c>
-      <c r="I6" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="K6">
-        <v>5</v>
-      </c>
-      <c r="L6" t="str">
-        <f t="shared" si="0"/>
-        <v>0.1uF</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="I6" t="s">
+        <v>338</v>
+      </c>
+      <c r="J6" s="44" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>252</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C7" s="45">
+        <v>0.1</v>
+      </c>
+      <c r="D7" s="45">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" t="s">
+        <v>311</v>
       </c>
       <c r="G7" t="s">
         <v>172</v>
@@ -2587,23 +2844,26 @@
       <c r="H7" t="s">
         <v>153</v>
       </c>
-      <c r="I7" s="43" t="s">
-        <v>171</v>
-      </c>
-      <c r="K7">
-        <v>5</v>
-      </c>
-      <c r="L7" t="str">
-        <f t="shared" si="0"/>
-        <v>47nF</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="I7" t="s">
+        <v>339</v>
+      </c>
+      <c r="J7" s="44" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>203</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="C8" s="45">
+        <v>0.15</v>
+      </c>
+      <c r="D8" s="45">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
       </c>
       <c r="E8" t="s">
         <v>87</v>
@@ -2612,808 +2872,1162 @@
         <v>93</v>
       </c>
       <c r="G8" t="s">
-        <v>204</v>
+        <v>285</v>
       </c>
       <c r="H8" t="s">
         <v>93</v>
       </c>
-      <c r="I8" s="43" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="J8" s="44" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>203</v>
+        <v>142</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="C9" s="45">
+        <v>0.83</v>
+      </c>
+      <c r="D9" s="45">
+        <f t="shared" si="0"/>
+        <v>3.32</v>
       </c>
       <c r="E9" t="s">
         <v>87</v>
       </c>
       <c r="F9" t="s">
-        <v>93</v>
+        <v>123</v>
       </c>
       <c r="G9" t="s">
-        <v>205</v>
+        <v>233</v>
       </c>
       <c r="H9" t="s">
-        <v>93</v>
-      </c>
-      <c r="I9" s="43" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+        <v>123</v>
+      </c>
+      <c r="J9" s="44" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>142</v>
+        <v>278</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
+      <c r="C10" s="45">
+        <v>3.19</v>
+      </c>
+      <c r="D10" s="45">
+        <f t="shared" si="0"/>
+        <v>6.38</v>
+      </c>
       <c r="E10" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="F10" t="s">
-        <v>123</v>
+        <v>214</v>
       </c>
       <c r="G10" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="H10" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
+        <v>215</v>
+      </c>
+      <c r="I10" t="s">
+        <v>279</v>
+      </c>
+      <c r="J10" s="44" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="C11" s="45">
+        <v>0.34</v>
+      </c>
+      <c r="D11" s="45">
+        <f t="shared" si="0"/>
+        <v>1.36</v>
       </c>
       <c r="E11" t="s">
-        <v>64</v>
+        <v>266</v>
       </c>
       <c r="F11" t="s">
-        <v>214</v>
+        <v>175</v>
       </c>
       <c r="G11" t="s">
-        <v>216</v>
+        <v>286</v>
       </c>
       <c r="H11" t="s">
-        <v>215</v>
-      </c>
-      <c r="I11" s="43" t="s">
-        <v>214</v>
-      </c>
-      <c r="L11" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
+        <v>154</v>
+      </c>
+      <c r="J11" s="44" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>265</v>
+        <v>234</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C12" s="45">
+        <v>0.21</v>
+      </c>
+      <c r="D12" s="45">
+        <f t="shared" si="0"/>
+        <v>0.42</v>
       </c>
       <c r="E12" t="s">
-        <v>266</v>
+        <v>235</v>
       </c>
       <c r="F12" t="s">
-        <v>175</v>
+        <v>236</v>
       </c>
       <c r="G12" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="H12" t="s">
-        <v>154</v>
-      </c>
-      <c r="I12" s="43" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
+        <v>143</v>
+      </c>
+      <c r="J12" s="44" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="C13" s="45">
+        <v>0.18</v>
+      </c>
+      <c r="D13" s="45">
+        <f t="shared" si="0"/>
+        <v>0.72</v>
       </c>
       <c r="E13" t="s">
         <v>266</v>
       </c>
       <c r="F13" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="G13" t="s">
-        <v>180</v>
+        <v>287</v>
       </c>
       <c r="H13" t="s">
         <v>154</v>
       </c>
-      <c r="I13" s="43" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="J13" s="44" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>234</v>
+        <v>268</v>
       </c>
       <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" s="45">
+        <v>0.17</v>
+      </c>
+      <c r="D14" s="45">
+        <f t="shared" si="0"/>
+        <v>0.34</v>
+      </c>
+      <c r="E14" t="s">
+        <v>266</v>
+      </c>
+      <c r="F14" t="s">
+        <v>183</v>
+      </c>
+      <c r="G14" t="s">
+        <v>288</v>
+      </c>
+      <c r="H14" t="s">
+        <v>154</v>
+      </c>
+      <c r="J14" s="44" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>211</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" s="45">
+        <v>5.95</v>
+      </c>
+      <c r="D15" s="45">
+        <f t="shared" si="0"/>
+        <v>11.9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>213</v>
+      </c>
+      <c r="F15" t="s">
+        <v>113</v>
+      </c>
+      <c r="G15" t="s">
+        <v>212</v>
+      </c>
+      <c r="H15" t="s">
+        <v>113</v>
+      </c>
+      <c r="J15" s="44" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>274</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16" s="45">
+        <v>2.1</v>
+      </c>
+      <c r="D16" s="45">
+        <f t="shared" si="0"/>
+        <v>8.4</v>
+      </c>
+      <c r="E16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" t="s">
+        <v>191</v>
+      </c>
+      <c r="H16" t="s">
+        <v>190</v>
+      </c>
+      <c r="J16" s="44" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>237</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" s="45">
+        <v>0.52</v>
+      </c>
+      <c r="D17" s="45">
+        <f t="shared" si="0"/>
+        <v>1.04</v>
+      </c>
+      <c r="E17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" t="s">
+        <v>209</v>
+      </c>
+      <c r="G17" t="s">
+        <v>210</v>
+      </c>
+      <c r="H17" t="s">
+        <v>207</v>
+      </c>
+      <c r="I17" t="s">
+        <v>238</v>
+      </c>
+      <c r="J17" s="44" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>239</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" s="45">
+        <v>0.42</v>
+      </c>
+      <c r="D18" s="45">
+        <f t="shared" si="0"/>
+        <v>0.84</v>
+      </c>
+      <c r="E18" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" t="s">
+        <v>206</v>
+      </c>
+      <c r="G18" t="s">
+        <v>208</v>
+      </c>
+      <c r="H18" t="s">
+        <v>207</v>
+      </c>
+      <c r="I18" t="s">
+        <v>240</v>
+      </c>
+      <c r="J18" s="44" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19" s="45">
+        <v>6.21</v>
+      </c>
+      <c r="D19" s="45">
+        <f t="shared" si="0"/>
+        <v>24.84</v>
+      </c>
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" t="s">
+        <v>243</v>
+      </c>
+      <c r="G19" t="s">
+        <v>241</v>
+      </c>
+      <c r="H19" t="s">
+        <v>192</v>
+      </c>
+      <c r="I19" t="s">
+        <v>242</v>
+      </c>
+      <c r="J19" s="44" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>197</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" s="45">
+        <v>31.42</v>
+      </c>
+      <c r="D20" s="45">
+        <f t="shared" si="0"/>
+        <v>62.84</v>
+      </c>
+      <c r="E20" t="s">
+        <v>200</v>
+      </c>
+      <c r="F20" t="s">
+        <v>197</v>
+      </c>
+      <c r="G20" t="s">
+        <v>199</v>
+      </c>
+      <c r="H20" t="s">
+        <v>198</v>
+      </c>
+      <c r="I20" t="s">
+        <v>244</v>
+      </c>
+      <c r="J20" s="44" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" s="45">
+        <v>52.25</v>
+      </c>
+      <c r="D21" s="45">
+        <f t="shared" si="0"/>
+        <v>104.5</v>
+      </c>
+      <c r="E21" t="s">
         <v>1</v>
       </c>
-      <c r="E14" t="s">
-        <v>235</v>
-      </c>
-      <c r="F14" t="s">
-        <v>236</v>
-      </c>
-      <c r="G14" t="s">
-        <v>144</v>
-      </c>
-      <c r="H14" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
-        <v>267</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>266</v>
-      </c>
-      <c r="F15" t="s">
-        <v>178</v>
-      </c>
-      <c r="G15" t="s">
-        <v>177</v>
-      </c>
-      <c r="H15" t="s">
-        <v>154</v>
-      </c>
-      <c r="I15" s="43" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
-        <v>267</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>266</v>
-      </c>
-      <c r="F16" t="s">
-        <v>178</v>
-      </c>
-      <c r="G16" t="s">
-        <v>187</v>
-      </c>
-      <c r="H16" t="s">
-        <v>154</v>
-      </c>
-      <c r="I16" s="43" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
-        <v>268</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>266</v>
-      </c>
-      <c r="F17" t="s">
-        <v>183</v>
-      </c>
-      <c r="G17" t="s">
-        <v>182</v>
-      </c>
-      <c r="H17" t="s">
-        <v>154</v>
-      </c>
-      <c r="I17" s="43" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
-        <v>268</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>266</v>
-      </c>
-      <c r="F18" t="s">
-        <v>183</v>
-      </c>
-      <c r="G18" t="s">
-        <v>185</v>
-      </c>
-      <c r="H18" t="s">
-        <v>154</v>
-      </c>
-      <c r="I18" s="43" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
-        <v>268</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="E19" t="s">
-        <v>266</v>
-      </c>
-      <c r="F19" t="s">
-        <v>183</v>
-      </c>
-      <c r="G19" t="s">
-        <v>194</v>
-      </c>
-      <c r="H19" t="s">
-        <v>154</v>
-      </c>
-      <c r="I19" s="43" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A20" t="s">
-        <v>268</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>266</v>
-      </c>
-      <c r="F20" t="s">
-        <v>183</v>
-      </c>
-      <c r="G20" t="s">
-        <v>196</v>
-      </c>
-      <c r="H20" t="s">
-        <v>154</v>
-      </c>
-      <c r="I20" s="43" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
-        <v>211</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>213</v>
-      </c>
       <c r="F21" t="s">
-        <v>113</v>
+        <v>34</v>
       </c>
       <c r="G21" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="H21" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
+        <v>201</v>
+      </c>
+      <c r="I21" t="s">
+        <v>276</v>
+      </c>
+      <c r="J21" s="44" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>274</v>
+        <v>249</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="C22" s="45">
+        <v>0.1</v>
+      </c>
+      <c r="D22" s="45">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
       </c>
       <c r="E22" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="F22" t="s">
-        <v>90</v>
+        <v>312</v>
       </c>
       <c r="G22" t="s">
-        <v>191</v>
+        <v>250</v>
       </c>
       <c r="H22" t="s">
-        <v>190</v>
-      </c>
-      <c r="I22" s="43" t="s">
-        <v>189</v>
-      </c>
-      <c r="J22" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.4">
+        <v>153</v>
+      </c>
+      <c r="I22" t="s">
+        <v>340</v>
+      </c>
+      <c r="J22" s="44" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="C23" s="45">
+        <v>0.1</v>
+      </c>
+      <c r="D23" s="45">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
       </c>
       <c r="E23" t="s">
         <v>73</v>
       </c>
       <c r="F23" t="s">
-        <v>209</v>
+        <v>317</v>
       </c>
       <c r="G23" t="s">
-        <v>210</v>
+        <v>254</v>
       </c>
       <c r="H23" t="s">
-        <v>207</v>
-      </c>
-      <c r="L23" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.4">
+        <v>153</v>
+      </c>
+      <c r="I23" t="s">
+        <v>341</v>
+      </c>
+      <c r="J23" s="44" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="B24">
+        <v>10</v>
+      </c>
+      <c r="C24" s="45">
+        <v>0.1</v>
+      </c>
+      <c r="D24" s="45">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E24" t="s">
         <v>73</v>
       </c>
       <c r="F24" t="s">
-        <v>206</v>
+        <v>316</v>
       </c>
       <c r="G24" t="s">
-        <v>208</v>
+        <v>257</v>
       </c>
       <c r="H24" t="s">
-        <v>207</v>
-      </c>
-      <c r="L24" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.4">
+        <v>153</v>
+      </c>
+      <c r="I24" t="s">
+        <v>342</v>
+      </c>
+      <c r="J24" s="44" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="B25">
         <v>2</v>
       </c>
+      <c r="C25" s="45">
+        <v>0.1</v>
+      </c>
+      <c r="D25" s="45">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25" t="s">
+        <v>322</v>
+      </c>
       <c r="G25" t="s">
-        <v>271</v>
+        <v>161</v>
       </c>
       <c r="H25" t="s">
-        <v>270</v>
-      </c>
-      <c r="I25" s="43" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.4">
+        <v>153</v>
+      </c>
+      <c r="I25" t="s">
+        <v>343</v>
+      </c>
+      <c r="J25" s="44" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>272</v>
+        <v>249</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="C26" s="45">
+        <v>0.1</v>
+      </c>
+      <c r="D26" s="45">
+        <f t="shared" si="0"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="E26" t="s">
+        <v>73</v>
+      </c>
+      <c r="F26" t="s">
+        <v>324</v>
       </c>
       <c r="G26" t="s">
-        <v>188</v>
+        <v>260</v>
       </c>
       <c r="H26" t="s">
-        <v>273</v>
-      </c>
-      <c r="I26" s="43" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.4">
+        <v>153</v>
+      </c>
+      <c r="I26" t="s">
+        <v>344</v>
+      </c>
+      <c r="J26" s="44" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>249</v>
       </c>
       <c r="B27">
         <v>2</v>
       </c>
+      <c r="C27" s="45">
+        <v>0.1</v>
+      </c>
+      <c r="D27" s="45">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
       <c r="E27" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="F27" t="s">
-        <v>243</v>
+        <v>325</v>
       </c>
       <c r="G27" t="s">
-        <v>241</v>
+        <v>167</v>
       </c>
       <c r="H27" t="s">
-        <v>192</v>
-      </c>
-      <c r="L27" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.4">
+        <v>153</v>
+      </c>
+      <c r="I27" t="s">
+        <v>345</v>
+      </c>
+      <c r="J27" s="44" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>197</v>
+        <v>249</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C28" s="45">
+        <v>0.1</v>
+      </c>
+      <c r="D28" s="45">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
       </c>
       <c r="E28" t="s">
-        <v>200</v>
+        <v>73</v>
       </c>
       <c r="F28" t="s">
-        <v>197</v>
+        <v>323</v>
       </c>
       <c r="G28" t="s">
-        <v>199</v>
+        <v>170</v>
       </c>
       <c r="H28" t="s">
-        <v>198</v>
-      </c>
-      <c r="J28">
-        <v>0.08</v>
-      </c>
-      <c r="L28" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.4">
+        <v>153</v>
+      </c>
+      <c r="I28" t="s">
+        <v>346</v>
+      </c>
+      <c r="J28" s="44" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>249</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="C29" s="45">
+        <v>0.1</v>
+      </c>
+      <c r="D29" s="45">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
       </c>
       <c r="E29" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="F29" t="s">
-        <v>34</v>
+        <v>327</v>
       </c>
       <c r="G29" t="s">
-        <v>202</v>
+        <v>263</v>
       </c>
       <c r="H29" t="s">
-        <v>201</v>
-      </c>
-      <c r="I29" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="L29" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.4">
+        <v>153</v>
+      </c>
+      <c r="I29" t="s">
+        <v>347</v>
+      </c>
+      <c r="J29" s="44" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>249</v>
       </c>
       <c r="B30">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="C30" s="45">
+        <v>0.1</v>
+      </c>
+      <c r="D30" s="45">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="E30" t="s">
+        <v>73</v>
+      </c>
+      <c r="F30" t="s">
+        <v>329</v>
       </c>
       <c r="G30" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="H30" t="s">
         <v>153</v>
       </c>
-      <c r="I30" s="43">
-        <v>0</v>
-      </c>
-      <c r="J30">
-        <v>0.125</v>
-      </c>
-      <c r="K30">
+      <c r="I30" t="s">
+        <v>348</v>
+      </c>
+      <c r="J30" s="44" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
+        <v>258</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" s="45">
+        <v>1.17</v>
+      </c>
+      <c r="D31" s="45">
+        <f t="shared" si="0"/>
+        <v>2.34</v>
+      </c>
+      <c r="E31" t="s">
+        <v>73</v>
+      </c>
+      <c r="F31" t="s">
+        <v>83</v>
+      </c>
+      <c r="G31" t="s">
+        <v>160</v>
+      </c>
+      <c r="H31" t="s">
+        <v>159</v>
+      </c>
+      <c r="I31" t="s">
+        <v>342</v>
+      </c>
+      <c r="J31" s="44" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>253</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32" s="45">
+        <v>0.79</v>
+      </c>
+      <c r="D32" s="45">
+        <f t="shared" si="0"/>
+        <v>1.58</v>
+      </c>
+      <c r="E32" t="s">
+        <v>73</v>
+      </c>
+      <c r="F32" t="s">
+        <v>331</v>
+      </c>
+      <c r="G32" t="s">
+        <v>155</v>
+      </c>
+      <c r="H32" t="s">
+        <v>154</v>
+      </c>
+      <c r="I32" t="s">
+        <v>349</v>
+      </c>
+      <c r="J32" s="44" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
+        <v>232</v>
+      </c>
+      <c r="B34">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A31" t="s">
-        <v>249</v>
-      </c>
-      <c r="B31">
-        <v>4</v>
-      </c>
-      <c r="G31" t="s">
-        <v>254</v>
-      </c>
-      <c r="H31" t="s">
-        <v>153</v>
-      </c>
-      <c r="I31" s="43">
-        <v>100</v>
-      </c>
-      <c r="J31">
-        <v>0.125</v>
-      </c>
-      <c r="K31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A32" t="s">
-        <v>249</v>
-      </c>
-      <c r="B32">
-        <v>5</v>
-      </c>
-      <c r="G32" t="s">
-        <v>257</v>
-      </c>
-      <c r="H32" t="s">
-        <v>153</v>
-      </c>
-      <c r="I32" s="43" t="s">
-        <v>158</v>
-      </c>
-      <c r="J32">
-        <v>0.125</v>
-      </c>
-      <c r="K32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A33" t="s">
-        <v>249</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="G33" t="s">
-        <v>161</v>
-      </c>
-      <c r="H33" t="s">
-        <v>153</v>
-      </c>
-      <c r="I33" s="43">
-        <v>137</v>
-      </c>
-      <c r="J33">
-        <v>0.125</v>
-      </c>
-      <c r="K33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A34" t="s">
-        <v>249</v>
-      </c>
-      <c r="B34">
-        <v>3</v>
+      <c r="C34" s="46">
+        <v>19.149999999999999</v>
+      </c>
+      <c r="D34" s="46">
+        <v>19.149999999999999</v>
+      </c>
+      <c r="E34" t="s">
+        <v>118</v>
+      </c>
+      <c r="F34" t="s">
+        <v>127</v>
       </c>
       <c r="G34" t="s">
-        <v>260</v>
+        <v>128</v>
       </c>
       <c r="H34" t="s">
-        <v>153</v>
-      </c>
-      <c r="I34" s="43">
-        <v>150</v>
-      </c>
-      <c r="J34">
-        <v>0.125</v>
-      </c>
-      <c r="K34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.4">
+        <v>129</v>
+      </c>
+      <c r="J34" s="44" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>249</v>
+        <v>9</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C35" s="46">
+        <v>39</v>
+      </c>
+      <c r="D35" s="46">
+        <v>78</v>
+      </c>
+      <c r="E35" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" t="s">
+        <v>26</v>
       </c>
       <c r="G35" t="s">
-        <v>167</v>
+        <v>8</v>
       </c>
       <c r="H35" t="s">
-        <v>153</v>
-      </c>
-      <c r="I35" s="43" t="s">
-        <v>166</v>
-      </c>
-      <c r="J35">
-        <v>0.125</v>
-      </c>
-      <c r="K35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.4">
+        <v>120</v>
+      </c>
+      <c r="I35" t="s">
+        <v>12</v>
+      </c>
+      <c r="J35" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>249</v>
+        <v>231</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C36" s="46">
+        <v>24</v>
+      </c>
+      <c r="D36" s="46">
+        <v>48</v>
+      </c>
+      <c r="E36" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" t="s">
+        <v>23</v>
       </c>
       <c r="G36" t="s">
-        <v>170</v>
+        <v>8</v>
       </c>
       <c r="H36" t="s">
-        <v>153</v>
-      </c>
-      <c r="I36" s="43" t="s">
-        <v>169</v>
-      </c>
-      <c r="J36">
-        <v>0.125</v>
-      </c>
-      <c r="K36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.4">
+        <v>19</v>
+      </c>
+      <c r="I36" t="s">
+        <v>15</v>
+      </c>
+      <c r="J36" s="44" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="B37">
         <v>2</v>
       </c>
+      <c r="C37" s="46">
+        <v>39</v>
+      </c>
+      <c r="D37" s="46">
+        <v>78</v>
+      </c>
+      <c r="E37" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" t="s">
+        <v>31</v>
+      </c>
       <c r="G37" t="s">
-        <v>263</v>
+        <v>8</v>
       </c>
       <c r="H37" t="s">
-        <v>153</v>
-      </c>
-      <c r="I37" s="43">
-        <v>68</v>
-      </c>
-      <c r="J37">
-        <v>0.125</v>
-      </c>
-      <c r="K37">
+        <v>19</v>
+      </c>
+      <c r="I37" t="s">
+        <v>17</v>
+      </c>
+      <c r="J37" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
+        <v>101</v>
+      </c>
+      <c r="B38">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A38" t="s">
-        <v>249</v>
-      </c>
-      <c r="B38">
+      <c r="C38" s="46">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="D38" s="46">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="E38" t="s">
+        <v>104</v>
+      </c>
+      <c r="F38" t="s">
+        <v>103</v>
+      </c>
+      <c r="G38" t="s">
+        <v>36</v>
+      </c>
+      <c r="H38" t="s">
+        <v>119</v>
+      </c>
+      <c r="I38" t="s">
+        <v>107</v>
+      </c>
+      <c r="J38" s="44" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
+        <v>282</v>
+      </c>
+      <c r="B39">
         <v>2</v>
       </c>
-      <c r="G38" t="s">
-        <v>264</v>
-      </c>
-      <c r="H38" t="s">
-        <v>153</v>
-      </c>
-      <c r="I38" s="43">
-        <v>82</v>
-      </c>
-      <c r="J38">
-        <v>0.125</v>
-      </c>
-      <c r="K38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A39" t="s">
-        <v>258</v>
-      </c>
-      <c r="B39">
-        <v>1</v>
+      <c r="C39" s="46">
+        <v>29.99</v>
+      </c>
+      <c r="D39" s="46">
+        <v>59.98</v>
       </c>
       <c r="E39" t="s">
-        <v>73</v>
+        <v>105</v>
       </c>
       <c r="F39" t="s">
-        <v>83</v>
+        <v>134</v>
       </c>
       <c r="G39" t="s">
-        <v>160</v>
+        <v>36</v>
       </c>
       <c r="H39" t="s">
-        <v>159</v>
-      </c>
-      <c r="I39" s="43" t="s">
-        <v>158</v>
-      </c>
-      <c r="J39">
-        <v>0.5</v>
-      </c>
-      <c r="K39">
-        <v>10</v>
-      </c>
-      <c r="L39" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.4">
+        <v>133</v>
+      </c>
+      <c r="J39" s="44" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C40" s="46">
+        <v>9.65</v>
+      </c>
+      <c r="D40" s="46">
+        <v>19.3</v>
+      </c>
+      <c r="E40" t="s">
+        <v>118</v>
+      </c>
+      <c r="F40" t="s">
+        <v>118</v>
       </c>
       <c r="G40" t="s">
-        <v>155</v>
+        <v>50</v>
       </c>
       <c r="H40" t="s">
-        <v>154</v>
-      </c>
-      <c r="I40" s="43">
+        <v>117</v>
+      </c>
+      <c r="I40" t="s">
+        <v>116</v>
+      </c>
+      <c r="J40" s="44" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>222</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41" s="46">
+        <v>0.41</v>
+      </c>
+      <c r="D41" s="46">
         <v>0.82</v>
       </c>
-      <c r="J40">
-        <v>0.5</v>
-      </c>
-      <c r="K40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A41" t="s">
-        <v>145</v>
-      </c>
-      <c r="B41">
-        <v>11</v>
+      <c r="E41" t="s">
+        <v>220</v>
+      </c>
+      <c r="F41" t="s">
+        <v>224</v>
       </c>
       <c r="G41" t="s">
-        <v>245</v>
-      </c>
-      <c r="H41" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.4">
+        <v>219</v>
+      </c>
+      <c r="J41" s="44" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>147</v>
+        <v>218</v>
       </c>
       <c r="B42">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C42" s="46">
+        <v>0.15</v>
+      </c>
+      <c r="D42" s="46">
+        <v>0.6</v>
+      </c>
+      <c r="E42" t="s">
+        <v>225</v>
+      </c>
+      <c r="F42">
+        <v>7682</v>
       </c>
       <c r="G42" t="s">
-        <v>246</v>
-      </c>
-      <c r="H42" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.4">
+        <v>219</v>
+      </c>
+      <c r="J42" s="44" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>149</v>
+        <v>227</v>
       </c>
       <c r="B43">
         <v>2</v>
       </c>
+      <c r="C43" s="46">
+        <v>0.13</v>
+      </c>
+      <c r="D43" s="46">
+        <v>0.26</v>
+      </c>
+      <c r="E43" t="s">
+        <v>225</v>
+      </c>
+      <c r="F43">
+        <v>4688</v>
+      </c>
       <c r="G43" t="s">
-        <v>247</v>
-      </c>
-      <c r="H43" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.4">
+        <v>219</v>
+      </c>
+      <c r="J43" s="44" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>151</v>
+        <v>228</v>
       </c>
       <c r="B44">
         <v>3</v>
       </c>
+      <c r="C44" s="46">
+        <v>3.95</v>
+      </c>
+      <c r="D44" s="46">
+        <v>11.850000000000001</v>
+      </c>
+      <c r="E44" t="s">
+        <v>139</v>
+      </c>
+      <c r="F44">
+        <v>1949</v>
+      </c>
       <c r="G44" t="s">
-        <v>248</v>
-      </c>
-      <c r="H44" t="s">
-        <v>152</v>
+        <v>88</v>
+      </c>
+      <c r="I44" t="s">
+        <v>138</v>
+      </c>
+      <c r="J44" s="44" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D45" s="6">
+        <f>SUM(D2:D44)</f>
+        <v>574.39</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J10" r:id="rId1"/>
+    <hyperlink ref="J8" r:id="rId2"/>
+    <hyperlink ref="J9" r:id="rId3"/>
+    <hyperlink ref="J11" r:id="rId4"/>
+    <hyperlink ref="J25" r:id="rId5"/>
+    <hyperlink ref="J29" r:id="rId6"/>
+    <hyperlink ref="J30" r:id="rId7"/>
+    <hyperlink ref="J31" r:id="rId8"/>
+    <hyperlink ref="J3" r:id="rId9"/>
+    <hyperlink ref="J4" r:id="rId10"/>
+    <hyperlink ref="J2" r:id="rId11"/>
+    <hyperlink ref="J5" r:id="rId12"/>
+    <hyperlink ref="J6" r:id="rId13"/>
+    <hyperlink ref="J7" r:id="rId14"/>
+    <hyperlink ref="J12" r:id="rId15"/>
+    <hyperlink ref="J13" r:id="rId16"/>
+    <hyperlink ref="J14" r:id="rId17"/>
+    <hyperlink ref="J15" r:id="rId18"/>
+    <hyperlink ref="J16" r:id="rId19"/>
+    <hyperlink ref="J17" r:id="rId20"/>
+    <hyperlink ref="J18" r:id="rId21"/>
+    <hyperlink ref="J19" r:id="rId22"/>
+    <hyperlink ref="J20" r:id="rId23"/>
+    <hyperlink ref="J21" r:id="rId24"/>
+    <hyperlink ref="J22" r:id="rId25"/>
+    <hyperlink ref="J24" r:id="rId26"/>
+    <hyperlink ref="J23" r:id="rId27"/>
+    <hyperlink ref="J26" r:id="rId28"/>
+    <hyperlink ref="J27" r:id="rId29"/>
+    <hyperlink ref="J28" r:id="rId30"/>
+    <hyperlink ref="J32" r:id="rId31"/>
+    <hyperlink ref="J34" r:id="rId32"/>
+    <hyperlink ref="J35" r:id="rId33"/>
+    <hyperlink ref="J36" r:id="rId34"/>
+    <hyperlink ref="J37" r:id="rId35"/>
+    <hyperlink ref="J38" r:id="rId36"/>
+    <hyperlink ref="J39" r:id="rId37"/>
+    <hyperlink ref="J40" r:id="rId38"/>
+    <hyperlink ref="J41" r:id="rId39"/>
+    <hyperlink ref="J42" r:id="rId40"/>
+    <hyperlink ref="J43" r:id="rId41"/>
+    <hyperlink ref="J44" r:id="rId42"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3422,7 +4036,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
@@ -4426,7 +5042,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4650,18 +5266,18 @@
     </row>
     <row r="7" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="12" t="s">
-        <v>135</v>
+        <v>282</v>
       </c>
       <c r="B7" s="13">
         <v>2</v>
       </c>
       <c r="C7" s="14">
-        <v>30</v>
+        <v>29.99</v>
       </c>
       <c r="D7" s="14">
         <f>Table13[[#This Row],[Quantity]]*Table13[[#This Row],[Cost
 (per unit)]]</f>
-        <v>60</v>
+        <v>59.98</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>105</v>
@@ -4689,13 +5305,12 @@
         <v>2</v>
       </c>
       <c r="C8" s="14">
-        <f>9.65 +4.99</f>
-        <v>14.64</v>
+        <v>9.65</v>
       </c>
       <c r="D8" s="14">
         <f>Table13[[#This Row],[Quantity]]*Table13[[#This Row],[Cost
 (per unit)]]</f>
-        <v>29.28</v>
+        <v>19.3</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>118</v>
@@ -4847,7 +5462,7 @@
       <c r="C13" s="28"/>
       <c r="D13" s="6">
         <f>SUM(D2:D12)</f>
-        <v>345.95</v>
+        <v>335.95000000000005</v>
       </c>
     </row>
   </sheetData>
@@ -4875,8 +5490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
fixes to silkscreen and gerber creation
</commit_message>
<xml_diff>
--- a/doc/design/bom.xlsx
+++ b/doc/design/bom.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="353">
   <si>
     <t>MFR</t>
   </si>
@@ -1078,6 +1078,15 @@
   </si>
   <si>
     <t>0.82Ω</t>
+  </si>
+  <si>
+    <t>SPT100H</t>
+  </si>
+  <si>
+    <t>Dimensions for top base are 1.75" x 1.25", 24 tooth spline (SPT100H) not the 25 tooth spline (SPT100F)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/445nm-405nm-Three-Element-Module/dp/B00B6EAJDM/ref=pd_sbs_267_1?_encoding=UTF8&amp;pd_rd_i=B00B6EAJDM&amp;pd_rd_r=QXSPH1ZFN11F0XFR9ARD&amp;pd_rd_w=qDJ8q&amp;pd_rd_wg=IJRUF&amp;psc=1&amp;refRID=QXSPH1ZFN11F0XFR9ARD</t>
   </si>
 </sst>
 </file>
@@ -2602,8 +2611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3793,7 +3802,7 @@
         <v>104</v>
       </c>
       <c r="F38" t="s">
-        <v>103</v>
+        <v>350</v>
       </c>
       <c r="G38" t="s">
         <v>36</v>
@@ -3802,7 +3811,7 @@
         <v>119</v>
       </c>
       <c r="I38" t="s">
-        <v>107</v>
+        <v>351</v>
       </c>
       <c r="J38" s="44" t="s">
         <v>102</v>
@@ -3845,7 +3854,7 @@
         <v>2</v>
       </c>
       <c r="C40" s="46">
-        <v>9.65</v>
+        <v>6.49</v>
       </c>
       <c r="D40" s="46">
         <v>19.3</v>
@@ -3866,7 +3875,7 @@
         <v>116</v>
       </c>
       <c r="J40" s="44" t="s">
-        <v>110</v>
+        <v>352</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.4">

</xml_diff>